<commit_message>
done work with sending siz to komplex
</commit_message>
<xml_diff>
--- a/template/akt-priema-peredachi-siz.xlsx
+++ b/template/akt-priema-peredachi-siz.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>АКТ</t>
   </si>
@@ -54,10 +54,16 @@
     <t>Принял:</t>
   </si>
   <si>
-    <t>_______________________________</t>
-  </si>
-  <si>
     <t>"___"____________ 20__ г.</t>
+  </si>
+  <si>
+    <t>Размер</t>
+  </si>
+  <si>
+    <t>Рост</t>
+  </si>
+  <si>
+    <t>____________________________</t>
   </si>
 </sst>
 </file>
@@ -130,7 +136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -156,6 +162,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -459,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I31"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,273 +479,398 @@
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="69" customWidth="1"/>
-    <col min="5" max="5" width="6.140625" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" customWidth="1"/>
+    <col min="7" max="7" width="5.28515625" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C2" s="2" t="s">
+    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C3" s="3" t="s">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="5" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="12" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B12" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C12" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="G12" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="H12" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="11"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
-      <c r="B16" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="B16" s="4"/>
       <c r="C16" s="4"/>
-      <c r="D16" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
-      <c r="B17" s="6" t="s">
-        <v>9</v>
-      </c>
+      <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="6" t="s">
-        <v>9</v>
-      </c>
+      <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
-      <c r="B19" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
-    </row>
-    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
+      <c r="B24" s="6"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G24" s="6"/>
+      <c r="H24" s="4"/>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
-    </row>
-    <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+    </row>
+    <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+    </row>
+    <row r="35" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>